<commit_message>
scores berekenen en toevoegen in de databank
</commit_message>
<xml_diff>
--- a/zoektermen_opdracht_sem1_sv.xlsx
+++ b/zoektermen_opdracht_sem1_sv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woutb\Documents\School\Data Engineering Project II\DEP_group_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD63AA3-E6A3-4BBC-94CC-DC62728F5984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40ACABD-CDF2-48CF-BB34-7EB65FF6E342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="276" windowWidth="23256" windowHeight="12792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -405,17 +405,17 @@
   </si>
   <si>
     <r>
-      <t>mensenrechten(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>leveranciers, afnemers), arbeidsrechten (leveranciers, afnemers), arbeidsomstandigheden (leveranciers, afnemers), kinderarbeid (leveranciers, afnemers), goede gezondheid en welzijn (leveranciers en werknemers), gezondheid (leveranciers, afnemers), welzijn (leveranciers, afnemers), rechten van werknemers, arbeisrechten, rechten en plichten van werknemers, arbeidsomstandigheden, algemene rechten en plichten, mensenrechten, recht op vrijheid,  gendergelijkheid (leveranciers, afnemers), waardig werk(leveranciers, afnemers), economische groei (leveranciers, afnemers),  ongelijkheid verminderen(leveranciers, afnemers), veiligheid(leveranciers, afnemers), waardeketen, lageloonlanden</t>
+      <t>mensenrechten (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>leveranciers/afnemers), arbeidsrechten (leveranciers/afnemers), arbeidsomstandigheden (leveranciers/afnemers), kinderarbeid (leveranciers/afnemers), goede gezondheid en welzijn (leveranciers/werknemers), gezondheid (leveranciers/afnemers), welzijn (leveranciers/afnemers), rechten van werknemers, arbeisrechten, rechten en plichten van werknemers, arbeidsomstandigheden, algemene rechten en plichten, mensenrechten, recht op vrijheid,  gendergelijkheid (leveranciers/afnemers), waardig werk (leveranciers/afnemers), economische groei (leveranciers/afnemers),  ongelijkheid verminderen (leveranciers/afnemers), veiligheid (leveranciers/afnemers), waardeketen, lageloonlanden</t>
     </r>
   </si>
 </sst>
@@ -1007,8 +1007,8 @@
   </sheetPr>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,7 +1088,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="282" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="131.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
@@ -1205,7 +1205,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>

</xml_diff>